<commit_message>
Atualização e criação de arquivos.
</commit_message>
<xml_diff>
--- a/certificates and licenses/Control/Control.xlsx
+++ b/certificates and licenses/Control/Control.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9e0d6736cb383cdc/Archives/2 - Github/licenses-and-certificates/Certificates/New control/Table control/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9e0d6736cb383cdc/Archives/2 - Github/licenses-and-certificates/certificates and licenses/Control/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="13_ncr:1_{AAD35425-F87E-4C11-9C09-CB5B2BB15EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17C82F78-1E1E-42EF-A16A-59B5A2C8D557}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="13_ncr:1_{AAD35425-F87E-4C11-9C09-CB5B2BB15EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AAD4F67-E2E4-4978-BE7C-FF1F63E6A982}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{63E668A9-ABAC-4246-A57F-81A0507FB8D7}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="101">
   <si>
     <t>Youtube parte 1: criação e otimização de um canal (de 03/02/2021 a 23/02/2021) 8hrs</t>
   </si>
@@ -326,6 +326,21 @@
   </si>
   <si>
     <t>https://cursos.alura.com.br/certificate/b9572da4-2224-4da1-b262-0931eb2c7d84</t>
+  </si>
+  <si>
+    <t>Aws</t>
+  </si>
+  <si>
+    <t>Governança de Dados</t>
+  </si>
+  <si>
+    <t>https://mycourse.app/MVxqobEMGb9Dp9LW6</t>
+  </si>
+  <si>
+    <t>AWS Certified Cloud Practitioner</t>
+  </si>
+  <si>
+    <t>https://www.credly.com/badges/38cdec31-4934-47a5-8da4-a51b01640397/linked_in_profile</t>
   </si>
 </sst>
 </file>
@@ -422,10 +437,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -725,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0F2FFB-C69B-48E5-8D17-73A3C2383ABD}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1863,6 +1874,58 @@
       </c>
       <c r="I44" s="3">
         <v>45154</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0</v>
+      </c>
+      <c r="E45" s="3">
+        <v>45187</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I45" s="3">
+        <v>45239</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B46" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46" s="2">
+        <v>8</v>
+      </c>
+      <c r="E46" s="3">
+        <v>45230</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I46" s="3">
+        <v>45239</v>
       </c>
     </row>
   </sheetData>
@@ -1911,8 +1974,10 @@
     <hyperlink ref="F42" r:id="rId39" xr:uid="{F92BB73A-4870-4463-9880-C0101089B75F}"/>
     <hyperlink ref="F43" r:id="rId40" xr:uid="{2200F868-1793-4044-8C8C-7509D9E3BC95}"/>
     <hyperlink ref="F44" r:id="rId41" xr:uid="{11373B3D-3505-4571-ACA3-186EAFF6C80D}"/>
+    <hyperlink ref="F46" r:id="rId42" xr:uid="{61BDC9B9-2D2F-42FD-A6A5-B4B8EF9DF595}"/>
+    <hyperlink ref="F45" r:id="rId43" xr:uid="{74FD30AE-E78C-4415-8107-09DCF86F78D4}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId42"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId44"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Criação e atualização de arquivos.
</commit_message>
<xml_diff>
--- a/certificates and licenses/Control/Control.xlsx
+++ b/certificates and licenses/Control/Control.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pheli\Desktop\Github\licenses-and-certificates\certificates and licenses\Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073E4EB2-00C6-4CC6-9574-3B6F6D86B292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53ED8F8-C203-4881-81B6-4BB99609F67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{63E668A9-ABAC-4246-A57F-81A0507FB8D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{63E668A9-ABAC-4246-A57F-81A0507FB8D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Control" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="119">
   <si>
     <t>Youtube parte 1: criação e otimização de um canal (de 03/02/2021 a 23/02/2021) 8hrs</t>
   </si>
@@ -350,6 +350,51 @@
   </si>
   <si>
     <t>Carlos Caldo Des. Profissional e Pessoal</t>
+  </si>
+  <si>
+    <t>Profissão Tech Lead: conhecendo a liderança técnica</t>
+  </si>
+  <si>
+    <t>https://cursos.alura.com.br/certificate/b4882cf7-e886-4d1a-9417-de87ff89c175</t>
+  </si>
+  <si>
+    <t>https://cursos.alura.com.br/certificate/571c0932-5061-4d7f-b53d-09c2f76858c8</t>
+  </si>
+  <si>
+    <t>Tech Lead: construindo práticas e rotinas de gestão</t>
+  </si>
+  <si>
+    <t>Associate - Analytics Engineering</t>
+  </si>
+  <si>
+    <t>https://www.brasilopenbadge.com.br/pages/badge/3311e6c17d9fcdf84d373e5da3ce2a65</t>
+  </si>
+  <si>
+    <t>Associate - Data Engineering</t>
+  </si>
+  <si>
+    <t>https://www.brasilopenbadge.com.br/pages/badge/1fafe09f5628c62e818a3d9a087f0900</t>
+  </si>
+  <si>
+    <t>Associate - Data Products</t>
+  </si>
+  <si>
+    <t>https://www.brasilopenbadge.com.br/pages/badge/3d69d5de91ef2bbb4ec8250cbf8ae683</t>
+  </si>
+  <si>
+    <t>Itaú (Open Badge)</t>
+  </si>
+  <si>
+    <t>Practitioner - Leadership D&amp;A</t>
+  </si>
+  <si>
+    <t>https://www.brasilopenbadge.com.br/pages/badge/e17f9d75f578a8ce0a61fa828c58fb6f</t>
+  </si>
+  <si>
+    <t>Practitioner - D&amp;A Foundation</t>
+  </si>
+  <si>
+    <t>https://www.brasilopenbadge.com.br/pages/badge/40f0aa1466bebed764160dd312179df2</t>
   </si>
 </sst>
 </file>
@@ -449,9 +494,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -489,7 +534,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -595,7 +640,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -737,7 +782,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -745,29 +790,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0F2FFB-C69B-48E5-8D17-73A3C2383ABD}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="86.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="0.88671875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1" hidden="1"/>
+    <col min="9" max="9" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="0.85546875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
@@ -793,7 +838,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>66</v>
       </c>
@@ -819,7 +864,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>65</v>
       </c>
@@ -845,7 +890,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>65</v>
       </c>
@@ -871,7 +916,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>66</v>
       </c>
@@ -897,7 +942,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -923,7 +968,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>27</v>
       </c>
@@ -949,7 +994,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
@@ -975,7 +1020,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
@@ -1001,7 +1046,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>66</v>
       </c>
@@ -1027,7 +1072,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
@@ -1053,7 +1098,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
@@ -1079,7 +1124,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
@@ -1105,7 +1150,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>27</v>
       </c>
@@ -1131,7 +1176,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>27</v>
       </c>
@@ -1157,7 +1202,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
@@ -1183,7 +1228,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>27</v>
       </c>
@@ -1209,7 +1254,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>27</v>
       </c>
@@ -1235,7 +1280,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
@@ -1261,7 +1306,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>27</v>
       </c>
@@ -1287,7 +1332,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>27</v>
       </c>
@@ -1313,7 +1358,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>27</v>
       </c>
@@ -1339,7 +1384,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>27</v>
       </c>
@@ -1365,7 +1410,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>58</v>
       </c>
@@ -1391,7 +1436,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
@@ -1417,7 +1462,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
@@ -1443,7 +1488,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>66</v>
       </c>
@@ -1469,7 +1514,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>27</v>
       </c>
@@ -1495,7 +1540,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>27</v>
       </c>
@@ -1521,7 +1566,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>27</v>
       </c>
@@ -1547,7 +1592,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>66</v>
       </c>
@@ -1573,7 +1618,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>66</v>
       </c>
@@ -1599,7 +1644,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
         <v>66</v>
       </c>
@@ -1625,7 +1670,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>27</v>
       </c>
@@ -1651,7 +1696,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>27</v>
       </c>
@@ -1677,7 +1722,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>27</v>
       </c>
@@ -1703,7 +1748,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>65</v>
       </c>
@@ -1729,7 +1774,7 @@
         <v>44744</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>65</v>
       </c>
@@ -1755,7 +1800,7 @@
         <v>44749</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>27</v>
       </c>
@@ -1781,7 +1826,7 @@
         <v>44753</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>27</v>
       </c>
@@ -1807,21 +1852,21 @@
         <v>44753</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
-        <v>65</v>
+        <v>114</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="D42" s="2">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E42" s="3">
-        <v>45078</v>
+        <v>44981</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>28</v>
@@ -1830,137 +1875,319 @@
         <v>28</v>
       </c>
       <c r="I42" s="3">
-        <v>45078</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+        <v>44981</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
-        <v>27</v>
+        <v>114</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="D43" s="2">
         <v>8</v>
       </c>
       <c r="E43" s="3">
+        <v>45104</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I43" s="3">
+        <v>45104</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D44" s="2">
+        <v>24</v>
+      </c>
+      <c r="E44" s="3">
+        <v>45078</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I44" s="3">
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="2">
+        <v>8</v>
+      </c>
+      <c r="E45" s="3">
         <v>45151</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F45" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I43" s="3">
+      <c r="G45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I45" s="3">
         <v>45151</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C44" s="2" t="s">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B46" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D46" s="2">
         <v>10</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E46" s="3">
         <v>45154</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F46" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="G44" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I44" s="3">
+      <c r="G46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I46" s="3">
         <v>45154</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="2" t="s">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B47" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D47" s="2">
         <v>0</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E47" s="3">
         <v>45187</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="F47" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="G45" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I45" s="3">
+      <c r="G47" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I47" s="3">
         <v>45239</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B48" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D48" s="2">
         <v>8</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E48" s="3">
         <v>45230</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="F48" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="G46" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I46" s="3">
+      <c r="G48" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I48" s="3">
         <v>45239</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="2" t="s">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B49" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D49" s="2">
         <v>24</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E49" s="3">
         <v>45227</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="F49" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="G47" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I47" s="3">
+      <c r="G49" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I49" s="3">
         <v>45227</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B50" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50" s="2">
+        <v>12</v>
+      </c>
+      <c r="E50" s="3">
+        <v>45322</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I50" s="3">
+        <v>45322</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B51" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D51" s="2">
+        <v>12</v>
+      </c>
+      <c r="E51" s="3">
+        <v>45322</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I51" s="3">
+        <v>45322</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B52" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D52" s="2">
+        <v>4</v>
+      </c>
+      <c r="E52" s="3">
+        <v>45322</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I52" s="3">
+        <v>45322</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B53" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D53" s="2">
+        <v>10</v>
+      </c>
+      <c r="E53" s="3">
+        <v>45388</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I53" s="3">
+        <v>45388</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B54" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" s="2">
+        <v>8</v>
+      </c>
+      <c r="E54" s="3">
+        <v>45388</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I54" s="3">
+        <v>45388</v>
       </c>
     </row>
   </sheetData>
@@ -2006,14 +2233,21 @@
     <hyperlink ref="F39" r:id="rId36" xr:uid="{24F14443-B5D3-497F-BB68-8932122C254B}"/>
     <hyperlink ref="F40" r:id="rId37" xr:uid="{3985EAEF-2E26-43A4-9767-4810C4F509AE}"/>
     <hyperlink ref="F41" r:id="rId38" xr:uid="{5EC806D4-4D6E-450F-B830-77F86AAB44F6}"/>
-    <hyperlink ref="F42" r:id="rId39" xr:uid="{F92BB73A-4870-4463-9880-C0101089B75F}"/>
-    <hyperlink ref="F43" r:id="rId40" xr:uid="{2200F868-1793-4044-8C8C-7509D9E3BC95}"/>
-    <hyperlink ref="F44" r:id="rId41" xr:uid="{11373B3D-3505-4571-ACA3-186EAFF6C80D}"/>
-    <hyperlink ref="F46" r:id="rId42" xr:uid="{61BDC9B9-2D2F-42FD-A6A5-B4B8EF9DF595}"/>
-    <hyperlink ref="F45" r:id="rId43" xr:uid="{74FD30AE-E78C-4415-8107-09DCF86F78D4}"/>
-    <hyperlink ref="F47" r:id="rId44" xr:uid="{D45705A3-046C-41D5-8586-11372C6D932B}"/>
+    <hyperlink ref="F44" r:id="rId39" xr:uid="{F92BB73A-4870-4463-9880-C0101089B75F}"/>
+    <hyperlink ref="F45" r:id="rId40" xr:uid="{2200F868-1793-4044-8C8C-7509D9E3BC95}"/>
+    <hyperlink ref="F46" r:id="rId41" xr:uid="{11373B3D-3505-4571-ACA3-186EAFF6C80D}"/>
+    <hyperlink ref="F48" r:id="rId42" xr:uid="{61BDC9B9-2D2F-42FD-A6A5-B4B8EF9DF595}"/>
+    <hyperlink ref="F47" r:id="rId43" xr:uid="{74FD30AE-E78C-4415-8107-09DCF86F78D4}"/>
+    <hyperlink ref="F49" r:id="rId44" xr:uid="{D45705A3-046C-41D5-8586-11372C6D932B}"/>
+    <hyperlink ref="F54" r:id="rId45" xr:uid="{BEE4A3C8-22E0-46D9-BEFF-1F0599BFF30C}"/>
+    <hyperlink ref="F53" r:id="rId46" xr:uid="{E93F6058-3102-442A-AF31-89FB6C967E95}"/>
+    <hyperlink ref="F50" r:id="rId47" xr:uid="{AAD584B6-B733-4A13-8CA0-3C2D93B77350}"/>
+    <hyperlink ref="F51" r:id="rId48" xr:uid="{31EAD665-6BB1-4A57-8DA4-828A856CB309}"/>
+    <hyperlink ref="F52" r:id="rId49" xr:uid="{8F644EFB-2A2A-4E80-AEDD-AC437938F2CE}"/>
+    <hyperlink ref="F42" r:id="rId50" xr:uid="{21C198E4-54BF-494C-94E0-937F7C6B2700}"/>
+    <hyperlink ref="F43" r:id="rId51" xr:uid="{A6F54A28-C025-4F41-BC45-1EB9655468E0}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId45"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId52"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Novos certificados e atualizações
</commit_message>
<xml_diff>
--- a/certificates and licenses/Control/Control.xlsx
+++ b/certificates and licenses/Control/Control.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pheli\Desktop\Github\licenses-and-certificates\certificates and licenses\Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1599E78-B08B-4D59-B993-99628CF371A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE25F4E-A72B-4E7E-8650-D07B6E786C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{63E668A9-ABAC-4246-A57F-81A0507FB8D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{63E668A9-ABAC-4246-A57F-81A0507FB8D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Control" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="135">
   <si>
     <t>Youtube parte 1: criação e otimização de um canal (de 03/02/2021 a 23/02/2021) 8hrs</t>
   </si>
@@ -419,6 +419,30 @@
   </si>
   <si>
     <t>https://cursos.alura.com.br/certificate/432decf7-933b-4c14-9ee7-7560b4078e30</t>
+  </si>
+  <si>
+    <t>Git e GitHub: compartilhando e colaborando em projetos</t>
+  </si>
+  <si>
+    <t>https://cursos.alura.com.br/certificate/3243a972-8425-49c5-aa70-3cb1141f23b1</t>
+  </si>
+  <si>
+    <t>Git e Github: controle e compartilhe seu código</t>
+  </si>
+  <si>
+    <t>Git e GitHub: repositório, commit e versões</t>
+  </si>
+  <si>
+    <t>https://cursos.alura.com.br/certificate/241bd285-12ed-4777-9175-2170a20e344d</t>
+  </si>
+  <si>
+    <t>https://cursos.alura.com.br/certificate/295511c8-6c4d-4c2f-a0b6-6f51d8146266</t>
+  </si>
+  <si>
+    <t>Git e GitHub: dominando controle de versão de código</t>
+  </si>
+  <si>
+    <t>https://cursos.alura.com.br/certificate/5f770eb3-4d2b-4f8c-9ef3-2aee95aa636a</t>
   </si>
 </sst>
 </file>
@@ -493,13 +517,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -815,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0F2FFB-C69B-48E5-8D17-73A3C2383ABD}">
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2267,7 +2290,7 @@
         <v>45395</v>
       </c>
     </row>
-    <row r="57" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57" s="2" t="s">
         <v>27</v>
       </c>
@@ -2280,7 +2303,7 @@
       <c r="E57" s="3">
         <v>45396</v>
       </c>
-      <c r="F57" s="5" t="s">
+      <c r="F57" s="4" t="s">
         <v>126</v>
       </c>
       <c r="G57" s="2" t="s">
@@ -2293,7 +2316,7 @@
         <v>45396</v>
       </c>
     </row>
-    <row r="58" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="s">
         <v>27</v>
       </c>
@@ -2306,7 +2329,7 @@
       <c r="E58" s="3">
         <v>45396</v>
       </c>
-      <c r="F58" s="5" t="s">
+      <c r="F58" s="4" t="s">
         <v>124</v>
       </c>
       <c r="G58" s="2" t="s">
@@ -2317,6 +2340,110 @@
       </c>
       <c r="I58" s="3">
         <v>45396</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B59" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D59" s="2">
+        <v>8</v>
+      </c>
+      <c r="E59" s="3">
+        <v>45397</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I59" s="3">
+        <v>45397</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B60" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D60" s="2">
+        <v>6</v>
+      </c>
+      <c r="E60" s="3">
+        <v>45397</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I60" s="3">
+        <v>45397</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B61" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D61" s="2">
+        <v>8</v>
+      </c>
+      <c r="E61" s="3">
+        <v>45397</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I61" s="3">
+        <v>45397</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B62" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D62" s="2">
+        <v>8</v>
+      </c>
+      <c r="E62" s="3">
+        <v>45397</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I62" s="3">
+        <v>45397</v>
       </c>
     </row>
   </sheetData>
@@ -2379,8 +2506,12 @@
     <hyperlink ref="F56" r:id="rId53" xr:uid="{5A8046BA-251C-4A4A-BF2F-B540D4A3BDC9}"/>
     <hyperlink ref="F58" r:id="rId54" xr:uid="{981E0DF0-8465-41E3-A9D9-A5CEE4716D22}"/>
     <hyperlink ref="F57" r:id="rId55" xr:uid="{58A820BC-D210-458D-94F6-500AC8C19D41}"/>
+    <hyperlink ref="F59" r:id="rId56" xr:uid="{A9454E4B-0BE7-4ED1-BD8B-6AD9D1F3636B}"/>
+    <hyperlink ref="F60" r:id="rId57" xr:uid="{2DDE640F-8C21-4C4E-9ED3-C8F1BD200D89}"/>
+    <hyperlink ref="F61" r:id="rId58" xr:uid="{0AFE3FE2-94DF-4EB8-B4F8-12EC55631F98}"/>
+    <hyperlink ref="F62" r:id="rId59" xr:uid="{4A96738B-C66F-46CA-84DA-902B4C5E7E66}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId56"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId60"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Criação de diretório e atualização de arquivo
</commit_message>
<xml_diff>
--- a/certificates and licenses/Control/Control.xlsx
+++ b/certificates and licenses/Control/Control.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pheli\Desktop\Github\licenses-and-certificates\certificates and licenses\Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pheli\Desktop\github\licenses-and-certificates\certificates and licenses\Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DA734D-4565-48C6-85AB-98279EB9BFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3393623-5B61-46AF-84ED-5CD7F7362B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{63E668A9-ABAC-4246-A57F-81A0507FB8D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{63E668A9-ABAC-4246-A57F-81A0507FB8D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Control" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="141">
   <si>
     <t>Youtube parte 1: criação e otimização de um canal (de 03/02/2021 a 23/02/2021) 8hrs</t>
   </si>
@@ -455,6 +455,12 @@
   </si>
   <si>
     <t>Spark: apresentando a ferramenta</t>
+  </si>
+  <si>
+    <t>Databricks: conhecendo a ferramenta</t>
+  </si>
+  <si>
+    <t>https://cursos.alura.com.br/certificate/f151e8d4-1a19-46ae-b002-ac909dafd7fd</t>
   </si>
 </sst>
 </file>
@@ -850,29 +856,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0F2FFB-C69B-48E5-8D17-73A3C2383ABD}">
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="86.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="0.88671875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1" hidden="1"/>
+    <col min="9" max="9" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="0.85546875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
@@ -898,7 +904,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>66</v>
       </c>
@@ -924,7 +930,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>65</v>
       </c>
@@ -950,7 +956,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>65</v>
       </c>
@@ -976,7 +982,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>66</v>
       </c>
@@ -1002,7 +1008,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -1028,7 +1034,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>27</v>
       </c>
@@ -1054,7 +1060,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
@@ -1080,7 +1086,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
@@ -1106,7 +1112,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>66</v>
       </c>
@@ -1132,7 +1138,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
@@ -1158,7 +1164,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
@@ -1184,7 +1190,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
@@ -1210,7 +1216,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>27</v>
       </c>
@@ -1236,7 +1242,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>27</v>
       </c>
@@ -1262,7 +1268,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
@@ -1288,7 +1294,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>27</v>
       </c>
@@ -1314,7 +1320,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>27</v>
       </c>
@@ -1340,7 +1346,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
@@ -1366,7 +1372,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>27</v>
       </c>
@@ -1392,7 +1398,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>27</v>
       </c>
@@ -1418,7 +1424,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>27</v>
       </c>
@@ -1444,7 +1450,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>27</v>
       </c>
@@ -1470,7 +1476,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>58</v>
       </c>
@@ -1496,7 +1502,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
@@ -1522,7 +1528,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
@@ -1548,7 +1554,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>66</v>
       </c>
@@ -1574,7 +1580,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>27</v>
       </c>
@@ -1600,7 +1606,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>27</v>
       </c>
@@ -1626,7 +1632,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>27</v>
       </c>
@@ -1652,7 +1658,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>66</v>
       </c>
@@ -1678,7 +1684,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>66</v>
       </c>
@@ -1704,7 +1710,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
         <v>66</v>
       </c>
@@ -1730,7 +1736,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>27</v>
       </c>
@@ -1756,7 +1762,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>27</v>
       </c>
@@ -1782,7 +1788,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>27</v>
       </c>
@@ -1808,7 +1814,7 @@
         <v>44712</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>65</v>
       </c>
@@ -1834,7 +1840,7 @@
         <v>44744</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>65</v>
       </c>
@@ -1860,7 +1866,7 @@
         <v>44749</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>27</v>
       </c>
@@ -1886,7 +1892,7 @@
         <v>44753</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>27</v>
       </c>
@@ -1912,7 +1918,7 @@
         <v>44753</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>114</v>
       </c>
@@ -1938,7 +1944,7 @@
         <v>44981</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
         <v>114</v>
       </c>
@@ -1964,7 +1970,7 @@
         <v>45104</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
         <v>65</v>
       </c>
@@ -1990,7 +1996,7 @@
         <v>45078</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
         <v>27</v>
       </c>
@@ -2016,7 +2022,7 @@
         <v>45151</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B46" s="2" t="s">
         <v>27</v>
       </c>
@@ -2042,7 +2048,7 @@
         <v>45154</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B47" s="2" t="s">
         <v>96</v>
       </c>
@@ -2068,7 +2074,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
         <v>65</v>
       </c>
@@ -2094,7 +2100,7 @@
         <v>45239</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
         <v>103</v>
       </c>
@@ -2120,7 +2126,7 @@
         <v>45227</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
         <v>114</v>
       </c>
@@ -2146,7 +2152,7 @@
         <v>45322</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
         <v>114</v>
       </c>
@@ -2172,7 +2178,7 @@
         <v>45322</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
         <v>114</v>
       </c>
@@ -2198,7 +2204,7 @@
         <v>45322</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B53" s="2" t="s">
         <v>27</v>
       </c>
@@ -2224,7 +2230,7 @@
         <v>45388</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B54" s="2" t="s">
         <v>27</v>
       </c>
@@ -2250,7 +2256,7 @@
         <v>45388</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="2" t="s">
         <v>66</v>
       </c>
@@ -2276,7 +2282,7 @@
         <v>45389</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B56" s="2" t="s">
         <v>66</v>
       </c>
@@ -2302,7 +2308,7 @@
         <v>45395</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57" s="2" t="s">
         <v>27</v>
       </c>
@@ -2328,7 +2334,7 @@
         <v>45396</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="s">
         <v>27</v>
       </c>
@@ -2354,7 +2360,7 @@
         <v>45396</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B59" s="2" t="s">
         <v>27</v>
       </c>
@@ -2380,7 +2386,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B60" s="2" t="s">
         <v>27</v>
       </c>
@@ -2406,7 +2412,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B61" s="2" t="s">
         <v>27</v>
       </c>
@@ -2432,7 +2438,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B62" s="2" t="s">
         <v>27</v>
       </c>
@@ -2458,7 +2464,7 @@
         <v>45397</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63" s="2" t="s">
         <v>27</v>
       </c>
@@ -2484,7 +2490,7 @@
         <v>45400</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B64" s="2" t="s">
         <v>27</v>
       </c>
@@ -2508,6 +2514,32 @@
       </c>
       <c r="I64" s="3">
         <v>45403</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B65" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D65" s="2">
+        <v>8</v>
+      </c>
+      <c r="E65" s="3">
+        <v>45435</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I65" s="3">
+        <v>45435</v>
       </c>
     </row>
   </sheetData>
@@ -2577,8 +2609,9 @@
     <hyperlink ref="F62" r:id="rId59" xr:uid="{4A96738B-C66F-46CA-84DA-902B4C5E7E66}"/>
     <hyperlink ref="F63" r:id="rId60" xr:uid="{C3FE1613-6A8A-4076-93AE-2FE719C9E1F4}"/>
     <hyperlink ref="F64" r:id="rId61" xr:uid="{59709705-CCC7-40DB-9824-FB35FC74DA1B}"/>
+    <hyperlink ref="F65" r:id="rId62" xr:uid="{2272C9B4-4C82-44CD-AC14-1F52CE0567E7}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId62"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId63"/>
 </worksheet>
 </file>
</xml_diff>